<commit_message>
Completed the code for new definition of M. Showed very interesting result. Now try to calculate <M^2> 's scaling with system size L.
</commit_message>
<xml_diff>
--- a/Bcrossing_graph/Fine_temp/Critical Temp.xlsx
+++ b/Bcrossing_graph/Fine_temp/Critical Temp.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UC Davis\Research\Synthetic Dimensions\Synthetic_dim_code\Bcrossing_graph\Fine_temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECE6211-F3FB-4629-BE80-EEC8CB37D925}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B10C33F-5D26-4D7C-A96B-6FF577E36CBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -33,7 +42,7 @@
     <t>Tc</t>
   </si>
   <si>
-    <t>0.84 missing</t>
+    <t>J0-J1</t>
   </si>
 </sst>
 </file>
@@ -160,7 +169,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -195,7 +204,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:f>Sheet1!$B$2:$B$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
@@ -345,7 +354,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$55</c:f>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
@@ -708,7 +717,1080 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>J0-J1 Intersection Plot</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.910207267257061E-2"/>
+          <c:y val="0.22293640218049668"/>
+          <c:w val="0.85391164233967154"/>
+          <c:h val="0.63607631738340398"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>0.622</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.60699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.60499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.60199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.59899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.59699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.59499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.59199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.58499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.58199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.57899999999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.57799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.57599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.57499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.57499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.57399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.57399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.57499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.57540000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.57599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.57799999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.57899999999999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.58250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.58399999999999996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.58699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.59099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.59499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.59799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.60099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.60499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.61399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.63500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.64500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.65500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8CEC-442B-AEEB-169063565802}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>J0-J1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.08</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.67999999999999994</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.65999999999999992</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.58000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.45999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.43999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.42000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.31999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.21999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.19999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.18000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9.9999999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.0000000000000053E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.0000000000000036E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.0000000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-2.0000000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-4.0000000000000036E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-6.0000000000000053E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-8.0000000000000071E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8CEC-442B-AEEB-169063565802}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="443329464"/>
+        <c:axId val="443324872"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="443329464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443324872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="443324872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443329464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1264,20 +2346,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>764381</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>173832</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>478631</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>59530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>154781</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>21432</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>261938</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1297,6 +2895,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>481012</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>128588</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D661EAE-F917-458E-9FFC-2D7E21B73394}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1570,436 +3204,652 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.796875" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" customWidth="1"/>
     <col min="3" max="3" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2">
+      <c r="B2">
         <v>0.622</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <f t="shared" ref="C2:C33" si="0">1-A2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
+        <v>0.02</v>
+      </c>
+      <c r="B3">
         <v>0.62</v>
       </c>
-      <c r="B3">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
+        <v>0.04</v>
+      </c>
+      <c r="B4">
         <v>0.61699999999999999</v>
       </c>
-      <c r="B4">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
+        <v>0.06</v>
+      </c>
+      <c r="B5">
         <v>0.61599999999999999</v>
       </c>
-      <c r="B5">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
+        <v>0.08</v>
+      </c>
+      <c r="B6">
         <v>0.61399999999999999</v>
       </c>
-      <c r="B6">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
+        <v>0.1</v>
+      </c>
+      <c r="B7">
         <v>0.61099999999999999</v>
       </c>
-      <c r="B7">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
+        <v>0.12</v>
+      </c>
+      <c r="B8">
         <v>0.60799999999999998</v>
       </c>
-      <c r="B8">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B9">
         <v>0.60699999999999998</v>
       </c>
-      <c r="B9">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
+        <v>0.16</v>
+      </c>
+      <c r="B10">
         <v>0.60499999999999998</v>
       </c>
-      <c r="B10">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
+        <v>0.18</v>
+      </c>
+      <c r="B11">
         <v>0.60199999999999998</v>
       </c>
-      <c r="B11">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.82000000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
+        <v>0.2</v>
+      </c>
+      <c r="B12">
         <v>0.59899999999999998</v>
       </c>
-      <c r="B12">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
+        <v>0.22</v>
+      </c>
+      <c r="B13">
         <v>0.59699999999999998</v>
       </c>
-      <c r="B13">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
+        <v>0.24</v>
+      </c>
+      <c r="B14">
         <v>0.59499999999999997</v>
       </c>
-      <c r="B14">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
+        <v>0.26</v>
+      </c>
+      <c r="B15">
         <v>0.59199999999999997</v>
       </c>
-      <c r="B15">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B16">
         <v>0.58899999999999997</v>
       </c>
-      <c r="B16">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
+        <v>0.3</v>
+      </c>
+      <c r="B17">
         <v>0.58699999999999997</v>
       </c>
-      <c r="B17">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
+        <v>0.32</v>
+      </c>
+      <c r="B18">
         <v>0.58499999999999996</v>
       </c>
-      <c r="B18">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.67999999999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
+        <v>0.34</v>
+      </c>
+      <c r="B19">
         <v>0.58199999999999996</v>
       </c>
-      <c r="B19">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.65999999999999992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
+        <v>0.36</v>
+      </c>
+      <c r="B20">
         <v>0.57899999999999996</v>
       </c>
-      <c r="B20">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
+        <v>0.38</v>
+      </c>
+      <c r="B21">
         <v>0.57799999999999996</v>
       </c>
-      <c r="B21">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
+        <v>0.4</v>
+      </c>
+      <c r="B22">
         <v>0.57599999999999996</v>
       </c>
-      <c r="B22">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>0.42</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.58000000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>0.44</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>0.46</v>
+      </c>
+      <c r="B25">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>0.48</v>
+      </c>
+      <c r="B26">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>0.5</v>
+      </c>
+      <c r="B27">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>0.52</v>
+      </c>
+      <c r="B28">
+        <v>0.57540000000000002</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>0.54</v>
+      </c>
+      <c r="B29">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0.45999999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B30">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0.43999999999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B31">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0.42000000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>0.6</v>
+      </c>
+      <c r="B32">
+        <v>0.58250000000000002</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
         <v>0.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="B23">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="1">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="B24">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="B25">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="B26">
-        <v>0.48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="B27">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>0.57540000000000002</v>
-      </c>
-      <c r="B28">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="B29">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="B30">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31">
-        <v>0.57899999999999996</v>
-      </c>
-      <c r="B31">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32">
-        <v>0.58250000000000002</v>
-      </c>
-      <c r="B32">
-        <v>0.6</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
+        <v>0.62</v>
+      </c>
+      <c r="B33">
         <v>0.58399999999999996</v>
       </c>
-      <c r="B33">
-        <v>0.62</v>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
+        <v>0.64</v>
+      </c>
+      <c r="B34">
         <v>0.58699999999999997</v>
       </c>
-      <c r="B34">
-        <v>0.64</v>
+      <c r="C34">
+        <f t="shared" ref="C34:C55" si="1">1-A34</f>
+        <v>0.36</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35">
+        <v>0.66</v>
+      </c>
+      <c r="B35">
         <v>0.59099999999999997</v>
       </c>
-      <c r="B35">
-        <v>0.66</v>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="1">
+      <c r="A36">
+        <v>0.68</v>
+      </c>
+      <c r="B36" s="1">
         <v>0.59499999999999997</v>
       </c>
-      <c r="B36">
-        <v>0.68</v>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>0.31999999999999995</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37">
+        <v>0.7</v>
+      </c>
+      <c r="B37">
         <v>0.59799999999999998</v>
       </c>
-      <c r="B37">
-        <v>0.7</v>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38">
+        <v>0.72</v>
+      </c>
+      <c r="B38">
         <v>0.60099999999999998</v>
       </c>
-      <c r="B38">
-        <v>0.72</v>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39">
+        <v>0.74</v>
+      </c>
+      <c r="B39">
         <v>0.60499999999999998</v>
       </c>
-      <c r="B39">
-        <v>0.74</v>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>0.26</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40">
+        <v>0.76</v>
+      </c>
+      <c r="B40">
         <v>0.61</v>
       </c>
-      <c r="B40">
-        <v>0.76</v>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41">
+        <v>0.78</v>
+      </c>
+      <c r="B41">
         <v>0.61399999999999999</v>
       </c>
-      <c r="B41">
-        <v>0.78</v>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>0.21999999999999997</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" s="1">
+      <c r="A42">
+        <v>0.8</v>
+      </c>
+      <c r="B42" s="1">
         <v>0.62</v>
       </c>
-      <c r="B42">
-        <v>0.8</v>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999996</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43">
+        <v>0.82</v>
+      </c>
+      <c r="B43">
         <v>0.625</v>
       </c>
-      <c r="B43">
-        <v>0.82</v>
-      </c>
-      <c r="C43" t="s">
-        <v>2</v>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>0.18000000000000005</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44">
+        <v>0.86</v>
+      </c>
+      <c r="B44">
         <v>0.63500000000000001</v>
       </c>
-      <c r="B44">
-        <v>0.86</v>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" s="1">
+      <c r="A45">
+        <v>0.88</v>
+      </c>
+      <c r="B45" s="1">
         <v>0.64500000000000002</v>
       </c>
-      <c r="B45">
-        <v>0.88</v>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" s="1">
+      <c r="A46">
+        <v>0.9</v>
+      </c>
+      <c r="B46" s="1">
         <v>0.65</v>
       </c>
-      <c r="B46">
-        <v>0.9</v>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" s="1">
+      <c r="A47">
+        <v>0.92</v>
+      </c>
+      <c r="B47" s="1">
         <v>0.65500000000000003</v>
       </c>
-      <c r="B47">
-        <v>0.92</v>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>7.999999999999996E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A48" s="1">
+      <c r="A48">
+        <v>0.94</v>
+      </c>
+      <c r="B48" s="1">
         <v>0.66</v>
       </c>
-      <c r="B48">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B49">
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000053E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B50">
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B51">
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B52">
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B53">
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>-2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53">
         <v>1.04</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B54">
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>-4.0000000000000036E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B55">
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>-6.0000000000000053E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55">
         <v>1.08</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>-8.0000000000000071E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mainly updated the plotting files and plots.
</commit_message>
<xml_diff>
--- a/Bcrossing_graph/Fine_temp/Critical Temp.xlsx
+++ b/Bcrossing_graph/Fine_temp/Critical Temp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UC Davis\Research\Synthetic Dimensions\Synthetic_dim_code\Bcrossing_graph\Fine_temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B10C33F-5D26-4D7C-A96B-6FF577E36CBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDA1E87-AAB2-4395-A17C-19953BCC5A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,6 +119,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Phase diagram on J-T plane</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -562,6 +587,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>T</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -624,6 +704,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>J1</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -690,9 +825,8 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
+        <a:schemeClr val="accent1">
+          <a:alpha val="96000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -3204,8 +3338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>